<commit_message>
added more example cases and minor model fixes
</commit_message>
<xml_diff>
--- a/emx/dist/urdm.xlsx
+++ b/emx/dist/urdm.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1044" uniqueCount="422">
   <si>
     <t>urdm</t>
   </si>
@@ -34,7 +34,7 @@
     <t>The Unified Rare Disease Model (URDM) for NGS data in research and healthcare (v0.9.2, 2021-11-16)</t>
   </si>
   <si>
-    <t>URDM Lookup tables (v0.9.2, 2021-11-16)</t>
+    <t>URDM Lookup tables (v0.9.3, 2021-11-16)</t>
   </si>
   <si>
     <t>dcat:catalog</t>
@@ -1037,6 +1037,9 @@
   </si>
   <si>
     <t>urdm_lookups_studyStatus</t>
+  </si>
+  <si>
+    <t>urdm_lookups_phenotype</t>
   </si>
   <si>
     <t>urdm_lookups_labIndication</t>
@@ -1650,16 +1653,16 @@
         <v>117</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>197</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1708,25 +1711,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>117</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>197</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -2077,7 +2080,7 @@
         <v>75</v>
       </c>
       <c r="G22" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -2160,37 +2163,37 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>117</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>197</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -4280,7 +4283,7 @@
         <v>144</v>
       </c>
       <c r="C71" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="D71" t="b">
         <v>0</v>
@@ -4299,6 +4302,9 @@
       </c>
       <c r="I71" t="b">
         <v>1</v>
+      </c>
+      <c r="J71" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="72" spans="1:10">
@@ -4309,7 +4315,7 @@
         <v>145</v>
       </c>
       <c r="C72" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="D72" t="b">
         <v>0</v>
@@ -4328,6 +4334,9 @@
       </c>
       <c r="I72" t="b">
         <v>1</v>
+      </c>
+      <c r="J72" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="73" spans="1:10">
@@ -4338,7 +4347,7 @@
         <v>146</v>
       </c>
       <c r="C73" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="D73" t="b">
         <v>0</v>
@@ -4357,6 +4366,9 @@
       </c>
       <c r="I73" t="b">
         <v>1</v>
+      </c>
+      <c r="J73" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="74" spans="1:10">
@@ -4812,7 +4824,7 @@
         <v>1</v>
       </c>
       <c r="J88" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="89" spans="1:11">
@@ -4960,7 +4972,7 @@
         <v>1</v>
       </c>
       <c r="J93" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="94" spans="1:11">
@@ -4992,7 +5004,7 @@
         <v>1</v>
       </c>
       <c r="J94" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="95" spans="1:11">
@@ -5024,7 +5036,7 @@
         <v>1</v>
       </c>
       <c r="J95" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="96" spans="1:11">
@@ -5901,7 +5913,7 @@
         <v>1</v>
       </c>
       <c r="J124" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="125" spans="1:11">
@@ -6107,7 +6119,7 @@
         <v>1</v>
       </c>
       <c r="J131" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="132" spans="1:11">
@@ -7290,22 +7302,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -7313,178 +7325,178 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="D2" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="E2" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B3" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="D3" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="E3" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B4" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="E4" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="B5" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="E5" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="B6" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="E6" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B7" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="E7" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B8" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="E8" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="B9" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="D9" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="E9" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B10" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="E10" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B11" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="E11" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -7492,294 +7504,294 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="D12" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="E12" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B13" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="D13" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="E13" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="B14" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="E14" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="B15" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="E15" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B16" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="E16" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="B17" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="E17" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B18" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="E18" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="B19" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="E19" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="B20" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="E20" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="B21" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="E21" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="B22" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="E22" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="B23" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="E23" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B24" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="E24" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="B25" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="E25" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B26" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="E26" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="B27" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="E27" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="B28" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="E28" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed attribute name: labProcedures (#10)
</commit_message>
<xml_diff>
--- a/emx/dist/urdm.xlsx
+++ b/emx/dist/urdm.xlsx
@@ -67,7 +67,7 @@
     <t>cohorts</t>
   </si>
   <si>
-    <t>laboratoryProcedures</t>
+    <t>labProcedures</t>
   </si>
   <si>
     <t>organizations</t>
@@ -448,7 +448,7 @@
     <t>urdm_cohorts</t>
   </si>
   <si>
-    <t>urdm_laboratoryProcedures</t>
+    <t>urdm_labProcedures</t>
   </si>
   <si>
     <t>urdm_organizations</t>
@@ -712,7 +712,7 @@
     <t>sequencingID</t>
   </si>
   <si>
-    <t>belongsTolabProcedure</t>
+    <t>belongsToLabProcedure</t>
   </si>
   <si>
     <t>belongsToSamplePreparation</t>

</xml_diff>